<commit_message>
Added more tutorial and document
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC53ED1-F6F6-4E9B-A974-1A9F018A766C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDAF03C-1E8B-436C-A28D-6FE03AFE9B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="type kinds" sheetId="1" r:id="rId1"/>
+    <sheet name="meta types" sheetId="1" r:id="rId1"/>
     <sheet name="canCast" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -916,17 +916,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,13 +940,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
-      </c>
-      <c r="F1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
       </c>
     </row>
@@ -973,7 +973,7 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
@@ -987,7 +987,7 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
@@ -1043,7 +1043,7 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0</v>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
@@ -1085,7 +1085,7 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0</v>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0</v>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0</v>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0</v>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0</v>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0</v>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0</v>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0</v>
       </c>
     </row>
@@ -1205,14 +1205,14 @@
       <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,10 +1225,10 @@
       <c r="C21" t="s">
         <v>99</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1240,13 +1240,13 @@
         <v>33</v>
       </c>
       <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F22" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="69" x14ac:dyDescent="0.25">
@@ -1256,14 +1256,14 @@
       <c r="B23">
         <v>34</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1273,14 +1273,14 @@
       <c r="B24">
         <v>35</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F24" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
@@ -1290,14 +1290,14 @@
       <c r="B25">
         <v>36</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1308,10 +1308,10 @@
         <v>37</v>
       </c>
       <c r="D26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" t="s">
         <v>96</v>
-      </c>
-      <c r="F26" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1321,11 +1321,11 @@
       <c r="B27">
         <v>38</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="D27" t="s">
         <v>115</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,14 +1335,14 @@
       <c r="B28">
         <v>39</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28">
         <v>1</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F28" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,10 +1352,10 @@
       <c r="B29">
         <v>40</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>1</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1366,14 +1366,14 @@
       <c r="B30">
         <v>41</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30">
         <v>1</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="F30" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,7 +1386,7 @@
       <c r="C31" t="s">
         <v>100</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>0</v>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       <c r="C32" t="s">
         <v>101</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>0</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       <c r="C33" t="s">
         <v>102</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>0</v>
       </c>
     </row>
@@ -1428,10 +1428,10 @@
       <c r="C34" t="s">
         <v>103</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1445,10 +1445,10 @@
       <c r="C35" t="s">
         <v>108</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>1</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1463,13 +1463,13 @@
         <v>109</v>
       </c>
       <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F36" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1482,14 +1482,14 @@
       <c r="C37" t="s">
         <v>110</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>104</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1502,14 +1502,14 @@
       <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>104</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1522,14 +1522,14 @@
       <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>104</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1542,14 +1542,14 @@
       <c r="C40" t="s">
         <v>120</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40">
         <v>1</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>104</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,14 +1562,14 @@
       <c r="C41" t="s">
         <v>121</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41">
         <v>1</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>104</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
       <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>0</v>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       <c r="C43" t="s">
         <v>124</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>0</v>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
       <c r="C44" t="s">
         <v>125</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>0</v>
       </c>
     </row>
@@ -1624,14 +1624,14 @@
       <c r="C45" t="s">
         <v>126</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45">
         <v>2</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
@@ -1644,14 +1644,14 @@
       <c r="C46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46">
         <v>2</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,14 +1664,14 @@
       <c r="C47" t="s">
         <v>129</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47">
         <v>1</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>130</v>
-      </c>
-      <c r="F47" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="69" x14ac:dyDescent="0.25">
@@ -1684,14 +1684,14 @@
       <c r="C48" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48">
         <v>1</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>130</v>
-      </c>
-      <c r="F48" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
@@ -1704,14 +1704,14 @@
       <c r="C49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49">
         <v>2</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
@@ -1724,14 +1724,14 @@
       <c r="C50" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50">
         <v>2</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
@@ -1744,14 +1744,14 @@
       <c r="C51" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51">
         <v>1</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>130</v>
-      </c>
-      <c r="F51" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
@@ -1764,14 +1764,14 @@
       <c r="C52" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E52">
         <v>1</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>130</v>
-      </c>
-      <c r="F52" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1784,14 +1784,14 @@
       <c r="C53" t="s">
         <v>131</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53">
         <v>1</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F53" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
@@ -1804,14 +1804,14 @@
       <c r="C54" t="s">
         <v>133</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" t="s">
         <v>134</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
       <c r="C55" t="s">
         <v>136</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>0</v>
       </c>
     </row>
@@ -1838,10 +1838,10 @@
       <c r="C56" t="s">
         <v>137</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed MetaMap to MetaMappable
</commit_message>
<xml_diff>
--- a/doc/tables.xlsx
+++ b/doc/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\metapp\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDAF03C-1E8B-436C-A28D-6FE03AFE9B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC3F8F0-FF3A-493C-B7B8-C57255088A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,11 +494,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MetaIterable
-MetaMap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>std::set&lt;Key, Compare, Allocator&gt;</t>
   </si>
   <si>
@@ -586,6 +581,10 @@
     Allocator
 &gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetaIterable
+MetaMappable</t>
   </si>
 </sst>
 </file>
@@ -917,7 +916,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1624,7 @@
         <v>126</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -1642,10 +1641,10 @@
         <v>84</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -1662,7 +1661,7 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
         <v>122</v>
@@ -1671,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="69" x14ac:dyDescent="0.25">
@@ -1682,7 +1681,7 @@
         <v>86</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
         <v>122</v>
@@ -1691,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="96.6" x14ac:dyDescent="0.25">
@@ -1702,10 +1701,10 @@
         <v>87</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -1722,10 +1721,10 @@
         <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -1742,7 +1741,7 @@
         <v>89</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
         <v>122</v>
@@ -1751,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
@@ -1762,7 +1761,7 @@
         <v>90</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
         <v>122</v>
@@ -1771,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
@@ -1782,7 +1781,7 @@
         <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D53" t="s">
         <v>118</v>
@@ -1791,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
@@ -1802,16 +1801,16 @@
         <v>92</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E54" t="s">
+        <v>133</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1822,7 +1821,7 @@
         <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1836,13 +1835,13 @@
         <v>94</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>